<commit_message>
added some stuff, not sure yet
</commit_message>
<xml_diff>
--- a/Marathontrainingsplan Felix.xlsx
+++ b/Marathontrainingsplan Felix.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Sport stuff\Trainingsplan Felix\gitrep felix\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED6355-43A1-46A2-9BA7-4B4BA8F163CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,127 +36,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="29">
-  <si>
-    <t xml:space="preserve">Marathontrainingsplan Felix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dienstag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mittwoch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donnerstag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freitag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samstag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonntag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aerobic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Race day</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="32">
+  <si>
+    <t>Marathontrainingsplan Felix</t>
+  </si>
+  <si>
+    <t>Woche 1</t>
+  </si>
+  <si>
+    <t>Montag</t>
+  </si>
+  <si>
+    <t>Dienstag</t>
+  </si>
+  <si>
+    <t>Mittwoch</t>
+  </si>
+  <si>
+    <t>Donnerstag</t>
+  </si>
+  <si>
+    <t>Freitag</t>
+  </si>
+  <si>
+    <t>Samstag</t>
+  </si>
+  <si>
+    <t>Sonntag</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Woche 2</t>
+  </si>
+  <si>
+    <t>Aerobic</t>
+  </si>
+  <si>
+    <t>Woche 3</t>
+  </si>
+  <si>
+    <t>Woche 4</t>
+  </si>
+  <si>
+    <t>Woche 5</t>
+  </si>
+  <si>
+    <t>Woche 6</t>
+  </si>
+  <si>
+    <t>Woche 7</t>
+  </si>
+  <si>
+    <t>Woche 8</t>
+  </si>
+  <si>
+    <t>Woche 9</t>
+  </si>
+  <si>
+    <t>Woche 10</t>
+  </si>
+  <si>
+    <t>Woche 11</t>
+  </si>
+  <si>
+    <t>Woche 12</t>
+  </si>
+  <si>
+    <t>Woche 13</t>
+  </si>
+  <si>
+    <t>Woche 14</t>
+  </si>
+  <si>
+    <t>Woche 15</t>
+  </si>
+  <si>
+    <t>Woche 16</t>
+  </si>
+  <si>
+    <t>Woche 17</t>
+  </si>
+  <si>
+    <t>Woche 18</t>
+  </si>
+  <si>
+    <t>Race day</t>
+  </si>
+  <si>
+    <t>4km einwärmen
+6 x (200m uphill 10k pace, 30s pause, 200m downhill mp)
+90s pause zwischen sets
+3km auslaufen</t>
+  </si>
+  <si>
+    <t>3km einwärmen
+2 x 3km hmp mit 3min joggen dazwischen
+3km auslaufen</t>
+  </si>
+  <si>
+    <t>11km easy
+10 x (1 min 10k pace, 1 min mp)
+3km easy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#&quot;km&quot;"/>
-    <numFmt numFmtId="166" formatCode="h:mm"/>
-    <numFmt numFmtId="167" formatCode="hh:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#&quot;km&quot;"/>
+    <numFmt numFmtId="165" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -187,15 +202,15 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="6">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF385724"/>
       </left>
@@ -210,7 +225,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF385724"/>
       </left>
@@ -223,7 +238,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF385724"/>
       </left>
@@ -238,78 +253,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF385724"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF385724"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF385724"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -368,40 +391,347 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.36"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -412,7 +742,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -435,22 +765,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="3">
         <v>6</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="3">
         <v>7</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I5" s="8">
+        <f>SUM(B5:H5)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
@@ -465,22 +799,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="6" t="n">
-        <v>0.03125</v>
+      <c r="D7" s="6">
+        <v>3.125E-2</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="6" t="n">
-        <v>0.0319444444444444</v>
+      <c r="F7" s="6">
+        <v>3.19444444444444E-2</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="6" t="n">
-        <v>0.04375</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H7" s="6">
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" ref="I6:I69" si="0">SUM(B7:H7)</f>
+        <v>0.1069444444444444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -488,9 +826,12 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -500,8 +841,9 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
@@ -523,25 +865,30 @@
       <c r="H11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="3">
         <v>8</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="3">
         <v>10</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3" t="n">
+      <c r="G12" s="3">
         <v>8</v>
       </c>
-      <c r="H12" s="3" t="n">
+      <c r="H12" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I12" s="8">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -554,36 +901,44 @@
       <c r="G13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="6" t="n">
-        <v>0.0416666666666667</v>
+      <c r="C14" s="6">
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="6" t="n">
-        <v>0.0402777777777778</v>
+      <c r="E14" s="6">
+        <v>4.0277777777777801E-2</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="8" t="n">
-        <v>0.0388888888888889</v>
-      </c>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G14" s="6">
+        <v>3.8888888888888903E-2</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1208333333333334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="11"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -593,8 +948,9 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -616,25 +972,30 @@
       <c r="H18" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="3">
         <v>10</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="3">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3" t="n">
+      <c r="G19" s="3">
         <v>10</v>
       </c>
-      <c r="H19" s="3" t="n">
+      <c r="H19" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I19" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -650,8 +1011,9 @@
       <c r="H20" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -659,8 +1021,12 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-    </row>
-    <row r="22" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I21" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -668,9 +1034,12 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
@@ -680,8 +1049,9 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
@@ -703,26 +1073,52 @@
       <c r="H25" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="3">
+        <v>12</v>
+      </c>
+      <c r="D26" s="3">
+        <v>7</v>
+      </c>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F26" s="3">
+        <v>11</v>
+      </c>
+      <c r="G26" s="3">
+        <v>6</v>
+      </c>
+      <c r="H26" s="3">
+        <v>21</v>
+      </c>
+      <c r="I26" s="8">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -730,8 +1126,12 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I28" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -739,9 +1139,12 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>14</v>
       </c>
@@ -751,8 +1154,9 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
@@ -774,26 +1178,48 @@
       <c r="H32" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="3">
+        <v>11</v>
+      </c>
       <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="E33" s="3">
+        <v>13</v>
+      </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G33" s="3">
+        <v>8</v>
+      </c>
+      <c r="H33" s="3">
+        <v>20</v>
+      </c>
+      <c r="I33" s="8">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="117.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="C34" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -801,8 +1227,12 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I35" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -810,9 +1240,12 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="1" t="s">
         <v>15</v>
       </c>
@@ -822,8 +1255,9 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
@@ -845,8 +1279,9 @@
       <c r="H39" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -854,8 +1289,12 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-    </row>
-    <row r="41" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I40" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -863,8 +1302,9 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -872,8 +1312,12 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
-    </row>
-    <row r="43" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I42" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -881,9 +1325,12 @@
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>16</v>
       </c>
@@ -893,8 +1340,9 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
@@ -916,8 +1364,9 @@
       <c r="H46" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -925,8 +1374,12 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-    </row>
-    <row r="48" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I47" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -934,8 +1387,9 @@
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I48" s="8"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -943,8 +1397,12 @@
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I49" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -952,9 +1410,12 @@
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I50" s="8"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>17</v>
       </c>
@@ -964,8 +1425,9 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-    </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I52" s="8"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
         <v>2</v>
       </c>
@@ -987,8 +1449,9 @@
       <c r="H53" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I53" s="8"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -996,8 +1459,12 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-    </row>
-    <row r="55" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I54" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -1005,8 +1472,9 @@
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-    </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I55" s="8"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -1014,8 +1482,12 @@
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-    </row>
-    <row r="57" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I56" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -1023,9 +1495,12 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I57" s="8"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I58" s="8"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" s="1" t="s">
         <v>18</v>
       </c>
@@ -1035,8 +1510,9 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I59" s="8"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
         <v>2</v>
       </c>
@@ -1058,8 +1534,9 @@
       <c r="H60" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I60" s="8"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -1067,8 +1544,12 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-    </row>
-    <row r="62" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I61" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -1076,8 +1557,9 @@
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -1085,8 +1567,12 @@
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
-    </row>
-    <row r="64" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I63" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -1094,9 +1580,12 @@
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I64" s="8"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I65" s="8"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B66" s="1" t="s">
         <v>19</v>
       </c>
@@ -1106,8 +1595,9 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-    </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I66" s="8"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B67" s="2" t="s">
         <v>2</v>
       </c>
@@ -1129,8 +1619,9 @@
       <c r="H67" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I67" s="8"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -1138,8 +1629,12 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-    </row>
-    <row r="69" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I68" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -1147,8 +1642,9 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
-    </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I69" s="8"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -1156,8 +1652,12 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
-    </row>
-    <row r="71" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I70" s="9">
+        <f t="shared" ref="I70:I127" si="1">SUM(B70:H70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -1165,9 +1665,12 @@
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I71" s="8"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I72" s="8"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B73" s="1" t="s">
         <v>20</v>
       </c>
@@ -1177,8 +1680,9 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
-    </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I73" s="8"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74" s="2" t="s">
         <v>2</v>
       </c>
@@ -1200,8 +1704,9 @@
       <c r="H74" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I74" s="8"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -1209,8 +1714,12 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
-    </row>
-    <row r="76" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I75" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -1218,8 +1727,9 @@
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
-    </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I76" s="8"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -1227,8 +1737,12 @@
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
-    </row>
-    <row r="78" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I77" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -1236,9 +1750,12 @@
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I78" s="8"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I79" s="8"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" s="1" t="s">
         <v>21</v>
       </c>
@@ -1248,8 +1765,9 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-    </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I80" s="8"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B81" s="2" t="s">
         <v>2</v>
       </c>
@@ -1271,8 +1789,9 @@
       <c r="H81" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I81" s="8"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -1280,8 +1799,12 @@
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-    </row>
-    <row r="83" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I82" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -1289,8 +1812,9 @@
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
-    </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I83" s="8"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -1298,8 +1822,12 @@
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
-    </row>
-    <row r="85" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I84" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -1307,9 +1835,12 @@
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I85" s="8"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I86" s="8"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B87" s="1" t="s">
         <v>22</v>
       </c>
@@ -1319,8 +1850,9 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
-    </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I87" s="8"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B88" s="2" t="s">
         <v>2</v>
       </c>
@@ -1342,8 +1874,9 @@
       <c r="H88" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I88" s="8"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -1351,8 +1884,12 @@
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
-    </row>
-    <row r="90" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I89" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
@@ -1360,8 +1897,9 @@
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
-    </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I90" s="8"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -1369,8 +1907,12 @@
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
-    </row>
-    <row r="92" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I91" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -1378,9 +1920,12 @@
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I92" s="8"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I93" s="8"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B94" s="1" t="s">
         <v>23</v>
       </c>
@@ -1390,8 +1935,9 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
-    </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I94" s="8"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B95" s="2" t="s">
         <v>2</v>
       </c>
@@ -1413,8 +1959,9 @@
       <c r="H95" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I95" s="8"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
@@ -1422,8 +1969,12 @@
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-    </row>
-    <row r="97" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I96" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
@@ -1431,8 +1982,9 @@
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
-    </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I97" s="8"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -1440,8 +1992,12 @@
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
-    </row>
-    <row r="99" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I98" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
@@ -1449,9 +2005,12 @@
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I99" s="8"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I100" s="8"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B101" s="1" t="s">
         <v>24</v>
       </c>
@@ -1461,8 +2020,9 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
-    </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I101" s="8"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B102" s="2" t="s">
         <v>2</v>
       </c>
@@ -1484,8 +2044,9 @@
       <c r="H102" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I102" s="8"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
@@ -1493,8 +2054,12 @@
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
-    </row>
-    <row r="104" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I103" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
@@ -1502,8 +2067,9 @@
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
-    </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I104" s="8"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -1511,8 +2077,12 @@
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
       <c r="H105" s="5"/>
-    </row>
-    <row r="106" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I105" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -1520,9 +2090,12 @@
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I106" s="8"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I107" s="8"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B108" s="1" t="s">
         <v>25</v>
       </c>
@@ -1532,8 +2105,9 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
-    </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I108" s="8"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B109" s="2" t="s">
         <v>2</v>
       </c>
@@ -1555,8 +2129,9 @@
       <c r="H109" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I109" s="8"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -1564,8 +2139,12 @@
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
-    </row>
-    <row r="111" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I110" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
@@ -1573,8 +2152,9 @@
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-    </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I111" s="8"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -1582,8 +2162,12 @@
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
       <c r="H112" s="5"/>
-    </row>
-    <row r="113" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I112" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
@@ -1591,9 +2175,12 @@
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I113" s="8"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I114" s="8"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B115" s="1" t="s">
         <v>26</v>
       </c>
@@ -1603,8 +2190,9 @@
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
-    </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I115" s="8"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B116" s="2" t="s">
         <v>2</v>
       </c>
@@ -1626,8 +2214,9 @@
       <c r="H116" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I116" s="8"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
@@ -1635,8 +2224,12 @@
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
-    </row>
-    <row r="118" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I117" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
@@ -1644,8 +2237,9 @@
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
-    </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I118" s="8"/>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -1653,8 +2247,12 @@
       <c r="F119" s="5"/>
       <c r="G119" s="5"/>
       <c r="H119" s="5"/>
-    </row>
-    <row r="120" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I119" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
@@ -1662,9 +2260,12 @@
       <c r="F120" s="7"/>
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
-    </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I120" s="8"/>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I121" s="8"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B122" s="1" t="s">
         <v>27</v>
       </c>
@@ -1674,8 +2275,9 @@
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
-    </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I122" s="8"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B123" s="2" t="s">
         <v>2</v>
       </c>
@@ -1697,8 +2299,9 @@
       <c r="H123" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I123" s="8"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
@@ -1708,8 +2311,12 @@
         <v>28</v>
       </c>
       <c r="H124" s="3"/>
-    </row>
-    <row r="125" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I124" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -1717,8 +2324,9 @@
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I125" s="8"/>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -1726,8 +2334,12 @@
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
-    </row>
-    <row r="127" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I126" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
@@ -1735,34 +2347,30 @@
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
+      <c r="I127" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B108:H108"/>
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="B122:H122"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B101:H101"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B66:H66"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="B17:H17"/>
     <mergeCell ref="B24:H24"/>
     <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B73:H73"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="B101:H101"/>
-    <mergeCell ref="B108:H108"/>
-    <mergeCell ref="B115:H115"/>
-    <mergeCell ref="B122:H122"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Time sum for week 2
</commit_message>
<xml_diff>
--- a/Marathontrainingsplan Felix.xlsx
+++ b/Marathontrainingsplan Felix.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Sport stuff\Trainingsplan Felix\gitrep felix\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B3E2E4-4591-4F0C-828B-F9D6CD59B72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -22,152 +38,134 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="34">
   <si>
-    <t xml:space="preserve">Marathontrainingsplan Felix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dienstag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mittwoch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donnerstag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freitag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samstag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonntag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aerobic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">280 hoehenmeter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450 hoehenmeter
+    <t>Marathontrainingsplan Felix</t>
+  </si>
+  <si>
+    <t>Woche 1</t>
+  </si>
+  <si>
+    <t>Montag</t>
+  </si>
+  <si>
+    <t>Dienstag</t>
+  </si>
+  <si>
+    <t>Mittwoch</t>
+  </si>
+  <si>
+    <t>Donnerstag</t>
+  </si>
+  <si>
+    <t>Freitag</t>
+  </si>
+  <si>
+    <t>Samstag</t>
+  </si>
+  <si>
+    <t>Sonntag</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Woche 2</t>
+  </si>
+  <si>
+    <t>Aerobic</t>
+  </si>
+  <si>
+    <t>280 hoehenmeter</t>
+  </si>
+  <si>
+    <t>450 hoehenmeter
 Esch ok gange
 Chli buchweh gha am 
 Morge, vo dem her 
 Ersch am abig gange</t>
   </si>
   <si>
-    <t xml:space="preserve">Woche 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4km einwärmen
+    <t>Woche 3</t>
+  </si>
+  <si>
+    <t>Woche 4</t>
+  </si>
+  <si>
+    <t>Woche 5</t>
+  </si>
+  <si>
+    <t>4km einwärmen
 6 x (200m uphill 10k pace, 30s pause, 200m downhill mp)
 90s pause zwischen sets
 3km auslaufen</t>
   </si>
   <si>
-    <t xml:space="preserve">3km einwärmen
+    <t>3km einwärmen
 2 x 3km hmp mit 3min joggen dazwischen
 3km auslaufen</t>
   </si>
   <si>
-    <t xml:space="preserve">11km easy
+    <t>11km easy
 10 x (1 min 10k pace, 1 min mp)
 3km easy</t>
   </si>
   <si>
-    <t xml:space="preserve">Woche 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woche 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Race day</t>
+    <t>Woche 6</t>
+  </si>
+  <si>
+    <t>Woche 7</t>
+  </si>
+  <si>
+    <t>Woche 8</t>
+  </si>
+  <si>
+    <t>Woche 9</t>
+  </si>
+  <si>
+    <t>Woche 10</t>
+  </si>
+  <si>
+    <t>Woche 11</t>
+  </si>
+  <si>
+    <t>Woche 12</t>
+  </si>
+  <si>
+    <t>Woche 13</t>
+  </si>
+  <si>
+    <t>Woche 14</t>
+  </si>
+  <si>
+    <t>Woche 15</t>
+  </si>
+  <si>
+    <t>Woche 16</t>
+  </si>
+  <si>
+    <t>Woche 17</t>
+  </si>
+  <si>
+    <t>Woche 18</t>
+  </si>
+  <si>
+    <t>Race day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#&quot;km&quot;"/>
-    <numFmt numFmtId="166" formatCode="h:mm"/>
-    <numFmt numFmtId="167" formatCode="hh:mm:ss"/>
-    <numFmt numFmtId="168" formatCode="@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#&quot;km&quot;"/>
+    <numFmt numFmtId="165" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -215,14 +213,14 @@
     </fill>
   </fills>
   <borders count="6">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF385724"/>
       </left>
@@ -237,7 +235,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF385724"/>
       </left>
@@ -250,7 +248,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF385724"/>
       </left>
@@ -265,7 +263,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF385724"/>
       </left>
@@ -278,109 +276,73 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="21" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -439,39 +401,347 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.36"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -482,7 +752,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -505,26 +775,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="3">
         <v>6</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="3">
         <v>7</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="3">
         <v>10</v>
       </c>
-      <c r="I5" s="4" t="n">
-        <f aca="false">SUM(B5:H5)</f>
+      <c r="I5" s="4">
+        <f>SUM(B5:H5)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -539,26 +809,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="7" t="n">
-        <v>0.03125</v>
+      <c r="D7" s="7">
+        <v>3.125E-2</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="7" t="n">
-        <v>0.0319444444444444</v>
+      <c r="F7" s="7">
+        <v>3.19444444444444E-2</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="7" t="n">
-        <v>0.04375</v>
-      </c>
-      <c r="I7" s="8" t="n">
-        <f aca="false">SUM(B7:H7)</f>
-        <v>0.106944444444444</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H7" s="7">
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="I7" s="8">
+        <f>SUM(B7:H7)</f>
+        <v>0.1069444444444444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -568,10 +838,10 @@
       <c r="H8" s="9"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -583,7 +853,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
@@ -607,28 +877,28 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="3">
         <v>8</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="3">
         <v>10</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3" t="n">
+      <c r="G12" s="3">
         <v>8</v>
       </c>
-      <c r="H12" s="3" t="n">
+      <c r="H12" s="3">
         <v>11</v>
       </c>
-      <c r="I12" s="4" t="n">
-        <f aca="false">SUM(B12:H12)</f>
+      <c r="I12" s="4">
+        <f>SUM(B12:H12)</f>
         <v>37</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -646,25 +916,28 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
-      <c r="C14" s="7" t="n">
-        <v>0.0416666666666667</v>
+      <c r="C14" s="7">
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="7" t="n">
-        <v>0.0402777777777778</v>
+      <c r="E14" s="7">
+        <v>4.0277777777777801E-2</v>
       </c>
       <c r="F14" s="6"/>
-      <c r="G14" s="7" t="n">
-        <v>0.0388888888888889</v>
-      </c>
-      <c r="H14" s="11" t="n">
-        <v>0.0555555555555556</v>
-      </c>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G14" s="7">
+        <v>3.8888888888888903E-2</v>
+      </c>
+      <c r="H14" s="11">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="I14" s="8">
+        <f>SUM(B14:H14)</f>
+        <v>0.17638888888888901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -678,10 +951,10 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -693,7 +966,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -717,28 +990,28 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="3">
         <v>10</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="3">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3" t="n">
+      <c r="G19" s="3">
         <v>10</v>
       </c>
-      <c r="H19" s="3" t="n">
+      <c r="H19" s="3">
         <v>18</v>
       </c>
-      <c r="I19" s="4" t="n">
-        <f aca="false">SUM(B19:H19)</f>
+      <c r="I19" s="4">
+        <f>SUM(B19:H19)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
         <v>9</v>
@@ -756,7 +1029,7 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -764,12 +1037,12 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="8" t="n">
-        <f aca="false">SUM(B21:H21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I21" s="8">
+        <f>SUM(B21:H21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -779,10 +1052,10 @@
       <c r="H22" s="9"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>15</v>
       </c>
@@ -794,7 +1067,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
@@ -818,30 +1091,30 @@
       </c>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="3">
         <v>12</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="3">
         <v>7</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="F26" s="3" t="n">
+      <c r="F26" s="3">
         <v>11</v>
       </c>
-      <c r="G26" s="3" t="n">
+      <c r="G26" s="3">
         <v>6</v>
       </c>
-      <c r="H26" s="3" t="n">
+      <c r="H26" s="3">
         <v>21</v>
       </c>
-      <c r="I26" s="4" t="n">
-        <f aca="false">SUM(B26:H26)</f>
+      <c r="I26" s="4">
+        <f>SUM(B26:H26)</f>
         <v>57</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
         <v>11</v>
@@ -861,7 +1134,7 @@
       </c>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -869,12 +1142,12 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="8" t="n">
-        <f aca="false">SUM(B28:H28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I28" s="8">
+        <f>SUM(B28:H28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -884,10 +1157,10 @@
       <c r="H29" s="9"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
@@ -899,7 +1172,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
@@ -923,28 +1196,28 @@
       </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="3">
         <v>11</v>
       </c>
       <c r="D33" s="3"/>
-      <c r="E33" s="3" t="n">
+      <c r="E33" s="3">
         <v>13</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="3" t="n">
+      <c r="G33" s="3">
         <v>8</v>
       </c>
-      <c r="H33" s="3" t="n">
+      <c r="H33" s="3">
         <v>20</v>
       </c>
-      <c r="I33" s="4" t="n">
-        <f aca="false">SUM(B33:H33)</f>
+      <c r="I33" s="4">
+        <f>SUM(B33:H33)</f>
         <v>52</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="2:9" ht="117" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="5"/>
       <c r="C34" s="13" t="s">
         <v>17</v>
@@ -962,7 +1235,7 @@
       </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -970,12 +1243,12 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="8" t="n">
-        <f aca="false">SUM(B35:H35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I35" s="8">
+        <f>SUM(B35:H35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -985,10 +1258,10 @@
       <c r="H36" s="9"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>20</v>
       </c>
@@ -1000,7 +1273,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1024,7 +1297,7 @@
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1032,12 +1305,12 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="4" t="n">
-        <f aca="false">SUM(B40:H40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I40" s="4">
+        <f>SUM(B40:H40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -1047,7 +1320,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -1055,12 +1328,12 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
-      <c r="I42" s="8" t="n">
-        <f aca="false">SUM(B42:H42)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I42" s="8">
+        <f>SUM(B42:H42)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
@@ -1070,10 +1343,10 @@
       <c r="H43" s="9"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1358,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
@@ -1109,7 +1382,7 @@
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1117,12 +1390,12 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="4" t="n">
-        <f aca="false">SUM(B47:H47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I47" s="4">
+        <f>SUM(B47:H47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1132,7 +1405,7 @@
       <c r="H48" s="5"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -1140,12 +1413,12 @@
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="8" t="n">
-        <f aca="false">SUM(B49:H49)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I49" s="8">
+        <f>SUM(B49:H49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
@@ -1155,10 +1428,10 @@
       <c r="H50" s="9"/>
       <c r="I50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>22</v>
       </c>
@@ -1170,7 +1443,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1467,7 @@
       </c>
       <c r="I53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -1202,12 +1475,12 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="4" t="n">
-        <f aca="false">SUM(B54:H54)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I54" s="4">
+        <f>SUM(B54:H54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -1217,7 +1490,7 @@
       <c r="H55" s="5"/>
       <c r="I55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
@@ -1225,12 +1498,12 @@
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
-      <c r="I56" s="8" t="n">
-        <f aca="false">SUM(B56:H56)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I56" s="8">
+        <f>SUM(B56:H56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -1240,10 +1513,10 @@
       <c r="H57" s="9"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" s="1" t="s">
         <v>23</v>
       </c>
@@ -1255,7 +1528,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
         <v>2</v>
       </c>
@@ -1279,7 +1552,7 @@
       </c>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -1287,12 +1560,12 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="4" t="n">
-        <f aca="false">SUM(B61:H61)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I61" s="4">
+        <f>SUM(B61:H61)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -1302,7 +1575,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="8"/>
     </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
@@ -1310,12 +1583,12 @@
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
-      <c r="I63" s="8" t="n">
-        <f aca="false">SUM(B63:H63)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I63" s="8">
+        <f>SUM(B63:H63)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
@@ -1325,10 +1598,10 @@
       <c r="H64" s="9"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B66" s="1" t="s">
         <v>24</v>
       </c>
@@ -1340,7 +1613,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B67" s="2" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1637,7 @@
       </c>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -1372,12 +1645,12 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="4" t="n">
-        <f aca="false">SUM(B68:H68)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I68" s="4">
+        <f>SUM(B68:H68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -1387,7 +1660,7 @@
       <c r="H69" s="5"/>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
@@ -1395,12 +1668,12 @@
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
-      <c r="I70" s="8" t="n">
-        <f aca="false">SUM(B70:H70)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I70" s="8">
+        <f>SUM(B70:H70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
@@ -1410,10 +1683,10 @@
       <c r="H71" s="9"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B73" s="1" t="s">
         <v>25</v>
       </c>
@@ -1425,7 +1698,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74" s="2" t="s">
         <v>2</v>
       </c>
@@ -1449,7 +1722,7 @@
       </c>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -1457,12 +1730,12 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
-      <c r="I75" s="4" t="n">
-        <f aca="false">SUM(B75:H75)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I75" s="4">
+        <f>SUM(B75:H75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -1472,7 +1745,7 @@
       <c r="H76" s="5"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
@@ -1480,12 +1753,12 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
-      <c r="I77" s="8" t="n">
-        <f aca="false">SUM(B77:H77)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I77" s="8">
+        <f>SUM(B77:H77)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
@@ -1495,10 +1768,10 @@
       <c r="H78" s="9"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I79" s="4"/>
     </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" s="1" t="s">
         <v>26</v>
       </c>
@@ -1510,7 +1783,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="4"/>
     </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B81" s="2" t="s">
         <v>2</v>
       </c>
@@ -1534,7 +1807,7 @@
       </c>
       <c r="I81" s="4"/>
     </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -1542,12 +1815,12 @@
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="4" t="n">
-        <f aca="false">SUM(B82:H82)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I82" s="4">
+        <f>SUM(B82:H82)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -1557,7 +1830,7 @@
       <c r="H83" s="5"/>
       <c r="I83" s="4"/>
     </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
@@ -1565,12 +1838,12 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
       <c r="H84" s="6"/>
-      <c r="I84" s="8" t="n">
-        <f aca="false">SUM(B84:H84)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I84" s="8">
+        <f>SUM(B84:H84)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
@@ -1580,10 +1853,10 @@
       <c r="H85" s="9"/>
       <c r="I85" s="4"/>
     </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I86" s="4"/>
     </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B87" s="1" t="s">
         <v>27</v>
       </c>
@@ -1595,7 +1868,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B88" s="2" t="s">
         <v>2</v>
       </c>
@@ -1619,7 +1892,7 @@
       </c>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -1627,12 +1900,12 @@
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
-      <c r="I89" s="4" t="n">
-        <f aca="false">SUM(B89:H89)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I89" s="4">
+        <f>SUM(B89:H89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -1642,7 +1915,7 @@
       <c r="H90" s="5"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
@@ -1650,12 +1923,12 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
-      <c r="I91" s="8" t="n">
-        <f aca="false">SUM(B91:H91)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I91" s="8">
+        <f>SUM(B91:H91)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
@@ -1665,10 +1938,10 @@
       <c r="H92" s="9"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I93" s="4"/>
     </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B94" s="1" t="s">
         <v>28</v>
       </c>
@@ -1680,7 +1953,7 @@
       <c r="H94" s="1"/>
       <c r="I94" s="4"/>
     </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B95" s="2" t="s">
         <v>2</v>
       </c>
@@ -1704,7 +1977,7 @@
       </c>
       <c r="I95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
@@ -1712,12 +1985,12 @@
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="I96" s="4" t="n">
-        <f aca="false">SUM(B96:H96)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I96" s="4">
+        <f>SUM(B96:H96)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -1727,7 +2000,7 @@
       <c r="H97" s="5"/>
       <c r="I97" s="4"/>
     </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
@@ -1735,12 +2008,12 @@
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
       <c r="H98" s="6"/>
-      <c r="I98" s="8" t="n">
-        <f aca="false">SUM(B98:H98)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I98" s="8">
+        <f>SUM(B98:H98)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
@@ -1750,10 +2023,10 @@
       <c r="H99" s="9"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I100" s="4"/>
     </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B101" s="1" t="s">
         <v>29</v>
       </c>
@@ -1765,7 +2038,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B102" s="2" t="s">
         <v>2</v>
       </c>
@@ -1789,7 +2062,7 @@
       </c>
       <c r="I102" s="4"/>
     </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
@@ -1797,12 +2070,12 @@
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
-      <c r="I103" s="4" t="n">
-        <f aca="false">SUM(B103:H103)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I103" s="4">
+        <f>SUM(B103:H103)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -1812,7 +2085,7 @@
       <c r="H104" s="5"/>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
@@ -1820,12 +2093,12 @@
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
       <c r="H105" s="6"/>
-      <c r="I105" s="8" t="n">
-        <f aca="false">SUM(B105:H105)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I105" s="8">
+        <f>SUM(B105:H105)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
@@ -1835,10 +2108,10 @@
       <c r="H106" s="9"/>
       <c r="I106" s="4"/>
     </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I107" s="4"/>
     </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B108" s="1" t="s">
         <v>30</v>
       </c>
@@ -1850,7 +2123,7 @@
       <c r="H108" s="1"/>
       <c r="I108" s="4"/>
     </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B109" s="2" t="s">
         <v>2</v>
       </c>
@@ -1874,7 +2147,7 @@
       </c>
       <c r="I109" s="4"/>
     </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -1882,12 +2155,12 @@
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
-      <c r="I110" s="4" t="n">
-        <f aca="false">SUM(B110:H110)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I110" s="4">
+        <f>SUM(B110:H110)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -1897,7 +2170,7 @@
       <c r="H111" s="5"/>
       <c r="I111" s="4"/>
     </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
@@ -1905,12 +2178,12 @@
       <c r="F112" s="6"/>
       <c r="G112" s="6"/>
       <c r="H112" s="6"/>
-      <c r="I112" s="8" t="n">
-        <f aca="false">SUM(B112:H112)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I112" s="8">
+        <f>SUM(B112:H112)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
       <c r="D113" s="9"/>
@@ -1920,10 +2193,10 @@
       <c r="H113" s="9"/>
       <c r="I113" s="4"/>
     </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I114" s="4"/>
     </row>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B115" s="1" t="s">
         <v>31</v>
       </c>
@@ -1935,7 +2208,7 @@
       <c r="H115" s="1"/>
       <c r="I115" s="4"/>
     </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B116" s="2" t="s">
         <v>2</v>
       </c>
@@ -1959,7 +2232,7 @@
       </c>
       <c r="I116" s="4"/>
     </row>
-    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
@@ -1967,12 +2240,12 @@
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
-      <c r="I117" s="4" t="n">
-        <f aca="false">SUM(B117:H117)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I117" s="4">
+        <f>SUM(B117:H117)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
@@ -1982,7 +2255,7 @@
       <c r="H118" s="5"/>
       <c r="I118" s="4"/>
     </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
@@ -1990,12 +2263,12 @@
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
       <c r="H119" s="6"/>
-      <c r="I119" s="8" t="n">
-        <f aca="false">SUM(B119:H119)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I119" s="8">
+        <f>SUM(B119:H119)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
       <c r="D120" s="9"/>
@@ -2005,10 +2278,10 @@
       <c r="H120" s="9"/>
       <c r="I120" s="4"/>
     </row>
-    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I121" s="4"/>
     </row>
-    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B122" s="1" t="s">
         <v>32</v>
       </c>
@@ -2020,7 +2293,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="4"/>
     </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B123" s="2" t="s">
         <v>2</v>
       </c>
@@ -2044,7 +2317,7 @@
       </c>
       <c r="I123" s="4"/>
     </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
@@ -2054,12 +2327,12 @@
         <v>33</v>
       </c>
       <c r="H124" s="3"/>
-      <c r="I124" s="4" t="n">
-        <f aca="false">SUM(B124:H124)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I124" s="4">
+        <f>SUM(B124:H124)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
@@ -2069,7 +2342,7 @@
       <c r="H125" s="5"/>
       <c r="I125" s="4"/>
     </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
       <c r="D126" s="6"/>
@@ -2077,12 +2350,12 @@
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
       <c r="H126" s="6"/>
-      <c r="I126" s="8" t="n">
-        <f aca="false">SUM(B126:H126)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I126" s="8">
+        <f>SUM(B126:H126)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
       <c r="D127" s="9"/>
@@ -2094,31 +2367,26 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B108:H108"/>
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="B122:H122"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B101:H101"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B66:H66"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="B17:H17"/>
     <mergeCell ref="B24:H24"/>
     <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B73:H73"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="B101:H101"/>
-    <mergeCell ref="B108:H108"/>
-    <mergeCell ref="B115:H115"/>
-    <mergeCell ref="B122:H122"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hemer s zistigstraining doch no usegnoh, für di <3
</commit_message>
<xml_diff>
--- a/Marathontrainingsplan Felix.xlsx
+++ b/Marathontrainingsplan Felix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Sport stuff\Trainingsplan Felix\gitrep felix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B3E2E4-4591-4F0C-828B-F9D6CD59B72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52407FDE-EF35-4C0B-9FF0-6E2DE3B5DAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="34">
   <si>
     <t>Marathontrainingsplan Felix</t>
   </si>
@@ -297,9 +297,6 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -336,6 +333,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,1631 +742,1637 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>6</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
         <v>7</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
         <v>10</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <f>SUM(B5:H5)</f>
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6">
         <v>3.125E-2</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7">
+      <c r="E7" s="5"/>
+      <c r="F7" s="6">
         <v>3.19444444444444E-2</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7">
+      <c r="G7" s="5"/>
+      <c r="H7" s="6">
         <v>4.3749999999999997E-2</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <f>SUM(B7:H7)</f>
         <v>0.1069444444444444</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="4"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="I9" s="4"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="4"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
         <v>8</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
         <v>10</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
         <v>8</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>11</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <f>SUM(B12:H12)</f>
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="6"/>
-      <c r="C14" s="7">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7">
+      <c r="D14" s="5"/>
+      <c r="E14" s="6">
         <v>4.0277777777777801E-2</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7">
+      <c r="F14" s="5"/>
+      <c r="G14" s="6">
         <v>3.8888888888888903E-2</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <v>5.5555555555555601E-2</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <f>SUM(B14:H14)</f>
         <v>0.17638888888888901</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="I16" s="4"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="4"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
         <v>10</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2">
         <v>12</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2">
         <v>10</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>18</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <f>SUM(B19:H19)</f>
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5" t="s">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="8">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="7">
         <f>SUM(B21:H21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="4"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I23" s="4"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="4"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="4"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2">
         <v>12</v>
       </c>
-      <c r="D26" s="3">
+      <c r="E26" s="2">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2">
+        <v>6</v>
+      </c>
+      <c r="H26" s="2">
+        <v>21</v>
+      </c>
+      <c r="I26" s="3">
+        <f>SUM(B26:H26)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="7">
+        <f>SUM(B28:H28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B31" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3">
+      <c r="H32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2">
         <v>11</v>
       </c>
-      <c r="G26" s="3">
-        <v>6</v>
-      </c>
-      <c r="H26" s="3">
-        <v>21</v>
-      </c>
-      <c r="I26" s="4">
-        <f>SUM(B26:H26)</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="8">
-        <f>SUM(B28:H28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="2" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2">
+        <v>13</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2">
         <v>8</v>
       </c>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3">
-        <v>11</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3">
-        <v>13</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3">
-        <v>8</v>
-      </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>20</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="3">
         <f>SUM(B33:H33)</f>
         <v>52</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="117" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="5"/>
-      <c r="C34" s="13" t="s">
+      <c r="B34" s="4"/>
+      <c r="C34" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="14" t="s">
+      <c r="D34" s="4"/>
+      <c r="E34" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5" t="s">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="I34" s="3"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="8">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="7">
         <f>SUM(B35:H35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="4"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="3"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I37" s="4"/>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="4"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="3"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I39" s="4"/>
+      <c r="I39" s="3"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="4">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="3">
         <f>SUM(B40:H40)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="3"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="8">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="7">
         <f>SUM(B42:H42)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="4"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="3"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I44" s="4"/>
+      <c r="I44" s="3"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="4"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="3"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I46" s="4"/>
+      <c r="I46" s="3"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="4">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="3">
         <f>SUM(B47:H47)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="3"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="8">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="7">
         <f>SUM(B49:H49)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="4"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="3"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I51" s="4"/>
+      <c r="I51" s="3"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="4"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="3"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="4"/>
+      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="4">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="3">
         <f>SUM(B54:H54)</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="3"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="8">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="7">
         <f>SUM(B56:H56)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="4"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="3"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I58" s="4"/>
+      <c r="I58" s="3"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="4"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="3"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I60" s="4"/>
+      <c r="I60" s="3"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="4">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="3">
         <f>SUM(B61:H61)</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="8"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="7"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="8">
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="7">
         <f>SUM(B63:H63)</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="4"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="3"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I65" s="4"/>
+      <c r="I65" s="3"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="4"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="3"/>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E67" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="H67" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I67" s="4"/>
+      <c r="I67" s="3"/>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="4">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="3">
         <f>SUM(B68:H68)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="3"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="8">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="7">
         <f>SUM(B70:H70)</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="4"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="3"/>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I72" s="4"/>
+      <c r="I72" s="3"/>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="4"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="3"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="H74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I74" s="4"/>
+      <c r="I74" s="3"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="4">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="3">
         <f>SUM(B75:H75)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="3"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="8">
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="7">
         <f>SUM(B77:H77)</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="4"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="3"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I79" s="4"/>
+      <c r="I79" s="3"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="4"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="3"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F81" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G81" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I81" s="4"/>
+      <c r="I81" s="3"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="4">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="3">
         <f>SUM(B82:H82)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="3"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
-      <c r="H84" s="6"/>
-      <c r="I84" s="8">
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="7">
         <f>SUM(B84:H84)</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-      <c r="H85" s="9"/>
-      <c r="I85" s="4"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="3"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I86" s="4"/>
+      <c r="I86" s="3"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="4"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="3"/>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E88" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G88" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="H88" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I88" s="4"/>
+      <c r="I88" s="3"/>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-      <c r="I89" s="4">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="3">
         <f>SUM(B89:H89)</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="3"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B91" s="6"/>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="6"/>
-      <c r="H91" s="6"/>
-      <c r="I91" s="8">
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="7">
         <f>SUM(B91:H91)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-      <c r="E92" s="9"/>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="H92" s="9"/>
-      <c r="I92" s="4"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="3"/>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I93" s="4"/>
+      <c r="I93" s="3"/>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="4"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="3"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D95" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="E95" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F95" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="G95" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H95" s="2" t="s">
+      <c r="H95" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I95" s="4"/>
+      <c r="I95" s="3"/>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="4">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="3">
         <f>SUM(B96:H96)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
-      <c r="I97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="3"/>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
-      <c r="F98" s="6"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="6"/>
-      <c r="I98" s="8">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="7">
         <f>SUM(B98:H98)</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="9"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="9"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="4"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="3"/>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I100" s="4"/>
+      <c r="I100" s="3"/>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="4"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="3"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B102" s="2" t="s">
+      <c r="B102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D102" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="E102" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F102" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G102" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="H102" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I102" s="4"/>
+      <c r="I102" s="3"/>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
-      <c r="H103" s="3"/>
-      <c r="I103" s="4">
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="3">
         <f>SUM(B103:H103)</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="3"/>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="8">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="7">
         <f>SUM(B105:H105)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="9"/>
-      <c r="C106" s="9"/>
-      <c r="D106" s="9"/>
-      <c r="E106" s="9"/>
-      <c r="F106" s="9"/>
-      <c r="G106" s="9"/>
-      <c r="H106" s="9"/>
-      <c r="I106" s="4"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="3"/>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I107" s="4"/>
+      <c r="I107" s="3"/>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="I108" s="4"/>
+      <c r="C108" s="14"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="14"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="3"/>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B109" s="2" t="s">
+      <c r="B109" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="D109" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="E109" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="F109" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="G109" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H109" s="2" t="s">
+      <c r="H109" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I109" s="4"/>
+      <c r="I109" s="3"/>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
-      <c r="G110" s="3"/>
-      <c r="H110" s="3"/>
-      <c r="I110" s="4">
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="3">
         <f>SUM(B110:H110)</f>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
-      <c r="G111" s="5"/>
-      <c r="H111" s="5"/>
-      <c r="I111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="3"/>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B112" s="6"/>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="6"/>
-      <c r="F112" s="6"/>
-      <c r="G112" s="6"/>
-      <c r="H112" s="6"/>
-      <c r="I112" s="8">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+      <c r="I112" s="7">
         <f>SUM(B112:H112)</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B113" s="9"/>
-      <c r="C113" s="9"/>
-      <c r="D113" s="9"/>
-      <c r="E113" s="9"/>
-      <c r="F113" s="9"/>
-      <c r="G113" s="9"/>
-      <c r="H113" s="9"/>
-      <c r="I113" s="4"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+      <c r="G113" s="8"/>
+      <c r="H113" s="8"/>
+      <c r="I113" s="3"/>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I114" s="4"/>
+      <c r="I114" s="3"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="4"/>
+      <c r="C115" s="14"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="14"/>
+      <c r="H115" s="14"/>
+      <c r="I115" s="3"/>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D116" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E116" s="2" t="s">
+      <c r="E116" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="F116" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="G116" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="H116" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I116" s="4"/>
+      <c r="I116" s="3"/>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
-      <c r="H117" s="3"/>
-      <c r="I117" s="4">
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="3">
         <f>SUM(B117:H117)</f>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
-      <c r="H118" s="5"/>
-      <c r="I118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="3"/>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B119" s="6"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="6"/>
-      <c r="F119" s="6"/>
-      <c r="G119" s="6"/>
-      <c r="H119" s="6"/>
-      <c r="I119" s="8">
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="7">
         <f>SUM(B119:H119)</f>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B120" s="9"/>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="4"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="8"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="8"/>
+      <c r="I120" s="3"/>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I121" s="4"/>
+      <c r="I121" s="3"/>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-      <c r="F122" s="1"/>
-      <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
-      <c r="I122" s="4"/>
+      <c r="C122" s="14"/>
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
+      <c r="F122" s="14"/>
+      <c r="G122" s="14"/>
+      <c r="H122" s="14"/>
+      <c r="I122" s="3"/>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D123" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E123" s="2" t="s">
+      <c r="E123" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F123" s="2" t="s">
+      <c r="F123" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G123" s="2" t="s">
+      <c r="G123" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H123" s="2" t="s">
+      <c r="H123" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I123" s="4"/>
+      <c r="I123" s="3"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
-      <c r="G124" s="3" t="s">
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H124" s="3"/>
-      <c r="I124" s="4">
+      <c r="H124" s="2"/>
+      <c r="I124" s="3">
         <f>SUM(B124:H124)</f>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5"/>
-      <c r="G125" s="5"/>
-      <c r="H125" s="5"/>
-      <c r="I125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="3"/>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B126" s="6"/>
-      <c r="C126" s="6"/>
-      <c r="D126" s="6"/>
-      <c r="E126" s="6"/>
-      <c r="F126" s="6"/>
-      <c r="G126" s="6"/>
-      <c r="H126" s="6"/>
-      <c r="I126" s="8">
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="5"/>
+      <c r="I126" s="7">
         <f>SUM(B126:H126)</f>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="2:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B127" s="9"/>
-      <c r="C127" s="9"/>
-      <c r="D127" s="9"/>
-      <c r="E127" s="9"/>
-      <c r="F127" s="9"/>
-      <c r="G127" s="9"/>
-      <c r="H127" s="9"/>
-      <c r="I127" s="4"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="8"/>
+      <c r="I127" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B66:H66"/>
     <mergeCell ref="B108:H108"/>
     <mergeCell ref="B115:H115"/>
     <mergeCell ref="B122:H122"/>
@@ -2375,16 +2381,6 @@
     <mergeCell ref="B87:H87"/>
     <mergeCell ref="B94:H94"/>
     <mergeCell ref="B101:H101"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B31:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>